<commit_message>
added several questions handeling and a tester
</commit_message>
<xml_diff>
--- a/qa.xlsx
+++ b/qa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dana Arad\Documents\comp2\web_data_mng\2022\hw2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomru\Documents\GitHub\WDM_Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69385C62-D52F-42EE-A42C-67CC2EFA9E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B634EA-6E4F-403C-B5A5-BC0800200B68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FE40923E-B6CD-43DC-ADCD-0AFB58BED0FB}"/>
+    <workbookView xWindow="-23040" yWindow="1044" windowWidth="23040" windowHeight="12204" xr2:uid="{FE40923E-B6CD-43DC-ADCD-0AFB58BED0FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -268,12 +268,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -288,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -299,6 +305,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -617,17 +626,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB5DB2EA-CAFF-4333-A57B-FF15E41828F8}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.26953125" customWidth="1"/>
-    <col min="2" max="2" width="45.54296875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="58.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.5546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -635,7 +644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -643,7 +652,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -651,7 +660,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -659,7 +668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -667,7 +676,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -675,7 +684,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -683,7 +692,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -691,7 +700,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -699,7 +708,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -707,15 +716,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -723,7 +732,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -731,7 +740,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -739,7 +748,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -747,15 +756,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
@@ -763,7 +772,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
@@ -771,15 +780,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>35</v>
       </c>
@@ -787,7 +796,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>42</v>
       </c>
@@ -795,7 +804,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>43</v>
       </c>
@@ -803,7 +812,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
@@ -811,15 +820,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>46</v>
       </c>
@@ -827,7 +836,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>47</v>
       </c>
@@ -835,7 +844,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>48</v>
       </c>
@@ -843,7 +852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>49</v>
       </c>
@@ -851,7 +860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>50</v>
       </c>
@@ -859,7 +868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>52</v>
       </c>
@@ -867,7 +876,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>57</v>
       </c>
@@ -875,7 +884,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>58</v>
       </c>
@@ -883,7 +892,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>60</v>
       </c>
@@ -891,7 +900,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>53</v>
       </c>
@@ -899,7 +908,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>63</v>
       </c>
@@ -907,7 +916,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>64</v>
       </c>
@@ -915,7 +924,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>65</v>
       </c>
@@ -923,16 +932,16 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="5"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
support for 'How many' questions + fixes
</commit_message>
<xml_diff>
--- a/qa.xlsx
+++ b/qa.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlust\Desktop\Project1\WDM_Project1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dana Arad\Documents\comp2\web_data_mng\2022\hw2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6175F7E5-F908-4150-9A92-C1F5C0917E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{115EFCCC-CC5A-4329-BFC7-01E6F27D421C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FE40923E-B6CD-43DC-ADCD-0AFB58BED0FB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FE40923E-B6CD-43DC-ADCD-0AFB58BED0FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>Who is the president of China?</t>
   </si>
@@ -100,7 +100,13 @@
     <t>Federal republic, Presidential system, Republic</t>
   </si>
   <si>
+    <t>84,069</t>
+  </si>
+  <si>
     <t>1,499</t>
+  </si>
+  <si>
+    <t>921,804</t>
   </si>
   <si>
     <t>What is the form of government in Sweden?</t>
@@ -271,18 +277,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -297,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -308,18 +308,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -638,13 +626,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB5DB2EA-CAFF-4333-A57B-FF15E41828F8}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="57.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.26953125" customWidth="1"/>
     <col min="2" max="2" width="45.54296875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
@@ -665,10 +653,10 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -692,8 +680,8 @@
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="8">
-        <v>84069</v>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -701,15 +689,15 @@
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="8">
-        <v>921804</v>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -746,137 +734,137 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>36</v>
+      <c r="A19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>47</v>
+      <c r="A21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>66</v>
+      <c r="A22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>67</v>
+      <c r="A23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>68</v>
+      <c r="A24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B25" s="1">
         <v>5</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B26" s="1">
         <v>5</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="6">
+      <c r="A27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="1">
         <v>2</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B28" s="1">
         <v>1</v>
@@ -884,7 +872,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
@@ -892,66 +880,66 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>